<commit_message>
2019 listo, trabajando con 2021
</commit_message>
<xml_diff>
--- a/preguntas/estructura/2019.xlsx
+++ b/preguntas/estructura/2019.xlsx
@@ -883,7 +883,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -905,10 +905,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1073,8 +1069,8 @@
   </sheetPr>
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1130,2497 +1126,2497 @@
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="9" t="n">
+      <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="9" t="n">
+      <c r="L2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="9" t="n">
+      <c r="I3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="9"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="9" t="n">
+      <c r="I4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="9" t="n">
+      <c r="L4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="8" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="9" t="n">
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="9" t="n">
+      <c r="I6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="9" t="n">
+      <c r="I7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="8" t="n">
         <v>5.16</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="9" t="n">
+      <c r="M7" s="8" t="n">
         <v>5.16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="9" t="n">
+      <c r="I8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="9" t="n">
+      <c r="I9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="8" t="n">
         <v>4.22</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="9" t="n">
+      <c r="M9" s="8" t="n">
         <v>4.22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="9" t="n">
+      <c r="I10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="9" t="n">
+      <c r="I11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="8" t="n">
         <v>5.84</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="9" t="n">
+      <c r="M11" s="8" t="n">
         <v>5.84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="J12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="9" t="n">
+      <c r="I13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="8" t="n">
         <v>4.78</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="9" t="n">
+      <c r="M13" s="8" t="n">
         <v>4.78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J14" s="9" t="n">
+      <c r="J14" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="K14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="9" t="n">
+      <c r="L14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="8" t="n">
         <v>3.78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="6"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="9" t="n">
+      <c r="I16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="8" t="n">
         <v>1.26</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="9" t="n">
+      <c r="L16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="8" t="n">
         <v>1.26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="s">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="9" t="n">
+      <c r="I17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="8" t="n">
         <v>1.26</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="6"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="9" t="n">
+      <c r="I18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="9" t="n">
+      <c r="L18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="8" t="n">
         <v>3.78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="9" t="n">
+      <c r="I19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="6"/>
+      <c r="M19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8" t="s">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="9" t="n">
+      <c r="I20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M20" s="6"/>
+      <c r="M20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8" t="s">
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="9" t="n">
+      <c r="I21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="6"/>
+      <c r="L21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="9" t="n">
+      <c r="I22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="6"/>
+      <c r="M22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="9" t="n">
+      <c r="J23" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="L23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" s="9" t="n">
+      <c r="L23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" s="8" t="n">
         <v>3.78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="9" t="n">
+      <c r="J24" s="8" t="n">
         <v>3.78</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="6"/>
+      <c r="M24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="9" t="n">
+      <c r="J25" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L25" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="6"/>
+      <c r="L25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8" t="s">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="9" t="n">
+      <c r="I26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M26" s="9" t="n">
+      <c r="M26" s="8" t="n">
         <v>4.2</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="9" t="n">
+      <c r="I27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M27" s="6"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8" t="s">
+      <c r="G28" s="7"/>
+      <c r="H28" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="9" t="n">
+      <c r="I28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="L28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M28" s="6"/>
+      <c r="L28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="9" t="n">
+      <c r="I29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="K29" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="L29" s="8" t="s">
+      <c r="L29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M29" s="6"/>
+      <c r="M29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="9" t="n">
+      <c r="I30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K30" s="8" t="s">
+      <c r="K30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="L30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="9" t="n">
+      <c r="L30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="8" t="n">
         <v>4.2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8" t="s">
+      <c r="G31" s="7"/>
+      <c r="H31" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="9" t="n">
+      <c r="I31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="K31" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="L31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M31" s="6"/>
+      <c r="M31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8" t="s">
+      <c r="G32" s="7"/>
+      <c r="H32" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="9" t="n">
+      <c r="I32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M32" s="6"/>
+      <c r="M32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="7" t="s">
+      <c r="A33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8" t="s">
+      <c r="C33" s="6"/>
+      <c r="D33" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8" t="s">
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I33" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="9" t="n">
+      <c r="I33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="K33" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L33" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M33" s="10"/>
+      <c r="L33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8" t="s">
+      <c r="G34" s="7"/>
+      <c r="H34" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="I34" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="9" t="n">
+      <c r="I34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="L34" s="8" t="s">
+      <c r="L34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8" t="s">
+      <c r="G35" s="7"/>
+      <c r="H35" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J35" s="9" t="n">
+      <c r="J35" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="L35" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M35" s="9" t="n">
+      <c r="L35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M35" s="8" t="n">
         <v>4.2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="8" t="s">
+      <c r="C36" s="6"/>
+      <c r="D36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J36" s="9" t="n">
+      <c r="J36" s="8" t="n">
         <v>4.2</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K36" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="L36" s="8" t="s">
+      <c r="L36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="10"/>
+      <c r="M36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8" t="s">
+      <c r="C37" s="6"/>
+      <c r="D37" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8" t="s">
+      <c r="G37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" s="9" t="n">
+      <c r="I37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="L37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M37" s="9" t="n">
+      <c r="L37" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="8" t="n">
         <v>10.8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8" t="s">
+      <c r="C38" s="6"/>
+      <c r="D38" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8" t="s">
+      <c r="E38" s="7"/>
+      <c r="F38" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8" t="s">
+      <c r="G38" s="7"/>
+      <c r="H38" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J38" s="9" t="n">
+      <c r="I38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="K38" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L38" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M38" s="10"/>
+      <c r="L38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8" t="s">
+      <c r="C39" s="6"/>
+      <c r="D39" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8" t="s">
+      <c r="G39" s="7"/>
+      <c r="H39" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" s="9" t="n">
+      <c r="I39" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L39" s="8" t="s">
+      <c r="L39" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M39" s="10"/>
+      <c r="M39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8" t="s">
+      <c r="C40" s="6"/>
+      <c r="D40" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8" t="s">
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8" t="s">
+      <c r="G40" s="7"/>
+      <c r="H40" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I40" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J40" s="9" t="n">
+      <c r="I40" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K40" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="L40" s="8" t="s">
+      <c r="L40" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M40" s="10"/>
+      <c r="M40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8" t="s">
+      <c r="C41" s="6"/>
+      <c r="D41" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8" t="s">
+      <c r="G41" s="7"/>
+      <c r="H41" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" s="9" t="n">
+      <c r="I41" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K41" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="L41" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M41" s="10"/>
+      <c r="M41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8" t="s">
+      <c r="C42" s="6"/>
+      <c r="D42" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
+      <c r="E42" s="7"/>
+      <c r="F42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8" t="s">
+      <c r="G42" s="7"/>
+      <c r="H42" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I42" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J42" s="9" t="n">
+      <c r="I42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="K42" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="L42" s="8" t="s">
+      <c r="L42" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M42" s="10"/>
+      <c r="M42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
+      <c r="E43" s="7"/>
+      <c r="F43" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8" t="s">
+      <c r="G43" s="7"/>
+      <c r="H43" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I43" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" s="9" t="n">
+      <c r="I43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K43" s="8" t="s">
+      <c r="K43" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L43" s="8" t="s">
+      <c r="L43" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M43" s="10"/>
+      <c r="M43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="7" t="s">
+      <c r="A44" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8" t="s">
+      <c r="C44" s="6"/>
+      <c r="D44" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8" t="s">
+      <c r="G44" s="7"/>
+      <c r="H44" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I44" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J44" s="9" t="n">
+      <c r="I44" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K44" s="8" t="s">
+      <c r="K44" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M44" s="10"/>
+      <c r="L44" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="7" t="s">
+      <c r="A45" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="8" t="s">
+      <c r="C45" s="6"/>
+      <c r="D45" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8" t="s">
+      <c r="G45" s="7"/>
+      <c r="H45" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" s="9" t="n">
+      <c r="I45" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K45" s="8" t="s">
+      <c r="K45" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="L45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M45" s="10"/>
+      <c r="L45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="7" t="s">
+      <c r="A46" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8" t="s">
+      <c r="C46" s="6"/>
+      <c r="D46" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8" t="s">
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8" t="s">
+      <c r="G46" s="7"/>
+      <c r="H46" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J46" s="9" t="n">
+      <c r="I46" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K46" s="8" t="s">
+      <c r="K46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="L46" s="8" t="s">
+      <c r="L46" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M46" s="10"/>
+      <c r="M46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="8" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8" t="s">
+      <c r="G47" s="7"/>
+      <c r="H47" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I47" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J47" s="9" t="n">
+      <c r="I47" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K47" s="8" t="s">
+      <c r="K47" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="L47" s="8" t="s">
+      <c r="L47" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M47" s="10"/>
+      <c r="M47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="8" t="s">
+      <c r="C48" s="6"/>
+      <c r="D48" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8" t="s">
+      <c r="E48" s="7"/>
+      <c r="F48" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8" t="s">
+      <c r="G48" s="7"/>
+      <c r="H48" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I48" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J48" s="9" t="n">
+      <c r="I48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K48" s="8" t="s">
+      <c r="K48" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="L48" s="8" t="s">
+      <c r="L48" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M48" s="10"/>
+      <c r="M48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8" t="s">
+      <c r="C49" s="6"/>
+      <c r="D49" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8" t="s">
+      <c r="G49" s="7"/>
+      <c r="H49" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I49" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J49" s="9" t="n">
+      <c r="I49" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" s="8" t="n">
         <v>10.8</v>
       </c>
-      <c r="K49" s="8" t="s">
+      <c r="K49" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L49" s="8" t="s">
+      <c r="L49" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M49" s="10"/>
+      <c r="M49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="7" t="s">
+      <c r="A50" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="8" t="s">
+      <c r="C50" s="6"/>
+      <c r="D50" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8" t="s">
+      <c r="E50" s="7"/>
+      <c r="F50" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8" t="s">
+      <c r="G50" s="7"/>
+      <c r="H50" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J50" s="9" t="n">
+      <c r="J50" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="K50" s="8" t="s">
+      <c r="K50" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="L50" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M50" s="9" t="n">
+      <c r="L50" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M50" s="8" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8" t="s">
+      <c r="C51" s="6"/>
+      <c r="D51" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8" t="s">
+      <c r="E51" s="7"/>
+      <c r="F51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8" t="s">
+      <c r="G51" s="7"/>
+      <c r="H51" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I51" s="8" t="s">
+      <c r="I51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J51" s="9" t="n">
+      <c r="J51" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="K51" s="8" t="s">
+      <c r="K51" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="L51" s="8" t="s">
+      <c r="L51" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M51" s="10"/>
+      <c r="M51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="7" t="s">
+      <c r="A52" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="8" t="s">
+      <c r="C52" s="6"/>
+      <c r="D52" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8" t="s">
+      <c r="E52" s="7"/>
+      <c r="F52" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8" t="s">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I52" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J52" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="K52" s="8" t="s">
+      <c r="I52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J52" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K52" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="L52" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M52" s="9" t="n">
+      <c r="L52" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M52" s="8" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="8" t="s">
+      <c r="C53" s="6"/>
+      <c r="D53" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8" t="s">
+      <c r="E53" s="7"/>
+      <c r="F53" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8" t="s">
+      <c r="G53" s="7"/>
+      <c r="H53" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J53" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="K53" s="8" t="s">
+      <c r="I53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K53" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="L53" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M53" s="9"/>
+      <c r="L53" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="8" t="s">
+      <c r="C54" s="6"/>
+      <c r="D54" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8" t="s">
+      <c r="E54" s="7"/>
+      <c r="F54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8" t="s">
+      <c r="G54" s="7"/>
+      <c r="H54" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I54" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J54" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="K54" s="8" t="s">
+      <c r="I54" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K54" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="L54" s="8" t="s">
+      <c r="L54" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M54" s="9"/>
+      <c r="M54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8" t="s">
+      <c r="E55" s="7"/>
+      <c r="F55" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8" t="s">
+      <c r="G55" s="7"/>
+      <c r="H55" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I55" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J55" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="K55" s="8" t="s">
+      <c r="I55" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K55" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="L55" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M55" s="9"/>
+      <c r="L55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="7" t="s">
+      <c r="A56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="8" t="s">
+      <c r="C56" s="6"/>
+      <c r="D56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8" t="s">
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8" t="s">
+      <c r="G56" s="7"/>
+      <c r="H56" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I56" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J56" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="K56" s="8" t="s">
+      <c r="I56" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="K56" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="L56" s="8" t="s">
+      <c r="L56" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M56" s="9"/>
+      <c r="M56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="7" t="s">
+      <c r="A57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8" t="s">
+      <c r="C57" s="6"/>
+      <c r="D57" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8" t="s">
+      <c r="E57" s="7"/>
+      <c r="F57" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8" t="s">
+      <c r="G57" s="7"/>
+      <c r="H57" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I57" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J57" s="9" t="n">
+      <c r="I57" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="K57" s="8" t="s">
+      <c r="K57" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="L57" s="8" t="s">
+      <c r="L57" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M57" s="9" t="n">
+      <c r="M57" s="8" t="n">
         <v>3.5</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="8" t="s">
+      <c r="C58" s="6"/>
+      <c r="D58" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8" t="s">
+      <c r="E58" s="7"/>
+      <c r="F58" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8" t="s">
+      <c r="G58" s="7"/>
+      <c r="H58" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I58" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J58" s="9" t="n">
+      <c r="I58" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="8" t="n">
         <v>1.5</v>
       </c>
-      <c r="K58" s="8" t="s">
+      <c r="K58" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="L58" s="8" t="s">
+      <c r="L58" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M58" s="9" t="n">
+      <c r="M58" s="8" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="8" t="s">
+      <c r="C59" s="6"/>
+      <c r="D59" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8" t="s">
+      <c r="E59" s="7"/>
+      <c r="F59" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8" t="s">
+      <c r="G59" s="7"/>
+      <c r="H59" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I59" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J59" s="9" t="n">
+      <c r="I59" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K59" s="8" t="s">
+      <c r="K59" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="L59" s="8"/>
-      <c r="M59" s="9" t="n">
+      <c r="L59" s="7"/>
+      <c r="M59" s="8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="8" t="s">
+      <c r="C60" s="6"/>
+      <c r="D60" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8" t="s">
+      <c r="E60" s="7"/>
+      <c r="F60" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8" t="s">
+      <c r="G60" s="7"/>
+      <c r="H60" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I60" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J60" s="9" t="n">
+      <c r="I60" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="K60" s="8" t="s">
+      <c r="K60" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="L60" s="8" t="s">
+      <c r="L60" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M60" s="9"/>
+      <c r="M60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="8" t="s">
+      <c r="C61" s="6"/>
+      <c r="D61" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8" t="s">
+      <c r="E61" s="7"/>
+      <c r="F61" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8" t="s">
+      <c r="G61" s="7"/>
+      <c r="H61" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="I61" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J61" s="9" t="n">
+      <c r="I61" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="8" t="n">
         <v>2.94</v>
       </c>
-      <c r="K61" s="8" t="s">
+      <c r="K61" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="L61" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M61" s="9" t="n">
+      <c r="L61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M61" s="8" t="n">
         <v>2.94</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="8" t="s">
+      <c r="C62" s="6"/>
+      <c r="D62" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8" t="s">
+      <c r="E62" s="7"/>
+      <c r="F62" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8" t="s">
+      <c r="G62" s="7"/>
+      <c r="H62" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="I62" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J62" s="9" t="n">
+      <c r="I62" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="8" t="n">
         <v>2.94</v>
       </c>
-      <c r="K62" s="8" t="s">
+      <c r="K62" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="L62" s="8" t="s">
+      <c r="L62" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M62" s="9"/>
+      <c r="M62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="8" t="s">
+      <c r="C63" s="6"/>
+      <c r="D63" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8" t="s">
+      <c r="E63" s="7"/>
+      <c r="F63" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8" t="s">
+      <c r="G63" s="7"/>
+      <c r="H63" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="I63" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" s="9" t="n">
+      <c r="I63" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" s="8" t="n">
         <v>0.78</v>
       </c>
-      <c r="K63" s="8" t="s">
+      <c r="K63" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="L63" s="8" t="s">
+      <c r="L63" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M63" s="9" t="n">
+      <c r="M63" s="8" t="n">
         <v>0.78</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="8" t="s">
+      <c r="C64" s="6"/>
+      <c r="D64" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8" t="s">
+      <c r="E64" s="7"/>
+      <c r="F64" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8" t="s">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I64" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J64" s="9" t="n">
+      <c r="I64" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J64" s="8" t="n">
         <v>0.78</v>
       </c>
-      <c r="K64" s="8" t="s">
+      <c r="K64" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="L64" s="8" t="s">
+      <c r="L64" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M64" s="9" t="n">
+      <c r="M64" s="8" t="n">
         <v>0.78</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="7" t="s">
+      <c r="A65" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8" t="s">
+      <c r="C65" s="6"/>
+      <c r="D65" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8" t="s">
+      <c r="E65" s="7"/>
+      <c r="F65" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8" t="s">
+      <c r="G65" s="7"/>
+      <c r="H65" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I65" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J65" s="9" t="n">
+      <c r="I65" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" s="8" t="n">
         <v>0.78</v>
       </c>
-      <c r="K65" s="8" t="s">
+      <c r="K65" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="L65" s="8" t="s">
+      <c r="L65" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M65" s="9" t="n">
+      <c r="M65" s="8" t="n">
         <v>0.78</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="7" t="s">
+      <c r="A66" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="8" t="s">
+      <c r="C66" s="6"/>
+      <c r="D66" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8" t="s">
+      <c r="E66" s="7"/>
+      <c r="F66" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8" t="s">
+      <c r="G66" s="7"/>
+      <c r="H66" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="I66" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="9" t="n">
+      <c r="I66" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K66" s="8" t="s">
+      <c r="K66" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="L66" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M66" s="9" t="n">
+      <c r="L66" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M66" s="8" t="n">
         <v>0.79</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="7" t="s">
+      <c r="A67" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="8" t="s">
+      <c r="C67" s="6"/>
+      <c r="D67" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8" t="s">
+      <c r="E67" s="7"/>
+      <c r="F67" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8" t="s">
+      <c r="G67" s="7"/>
+      <c r="H67" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I67" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="9" t="n">
+      <c r="I67" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K67" s="8" t="s">
+      <c r="K67" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="L67" s="8" t="s">
+      <c r="L67" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M67" s="9" t="n">
+      <c r="M67" s="8" t="n">
         <v>0.79</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B68" s="7" t="s">
+      <c r="A68" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="8" t="s">
+      <c r="C68" s="6"/>
+      <c r="D68" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8" t="s">
+      <c r="E68" s="7"/>
+      <c r="F68" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8" t="s">
+      <c r="G68" s="7"/>
+      <c r="H68" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I68" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J68" s="9" t="n">
+      <c r="I68" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J68" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K68" s="8" t="s">
+      <c r="K68" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="L68" s="8" t="s">
+      <c r="L68" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M68" s="9"/>
+      <c r="M68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="7" t="s">
+      <c r="A69" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="8" t="s">
+      <c r="C69" s="6"/>
+      <c r="D69" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8" t="s">
+      <c r="E69" s="7"/>
+      <c r="F69" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8" t="s">
+      <c r="G69" s="7"/>
+      <c r="H69" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I69" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J69" s="9" t="n">
+      <c r="I69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J69" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K69" s="8" t="s">
+      <c r="K69" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="L69" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M69" s="9"/>
+      <c r="L69" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="7" t="s">
+      <c r="A70" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="8" t="s">
+      <c r="C70" s="6"/>
+      <c r="D70" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8" t="s">
+      <c r="E70" s="7"/>
+      <c r="F70" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8" t="s">
+      <c r="G70" s="7"/>
+      <c r="H70" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="I70" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J70" s="9" t="n">
+      <c r="I70" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J70" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K70" s="8" t="s">
+      <c r="K70" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="L70" s="8" t="s">
+      <c r="L70" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M70" s="9"/>
+      <c r="M70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="7"/>
-      <c r="D71" s="8" t="s">
+      <c r="C71" s="6"/>
+      <c r="D71" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8" t="s">
+      <c r="E71" s="7"/>
+      <c r="F71" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8" t="s">
+      <c r="G71" s="7"/>
+      <c r="H71" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I71" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J71" s="9" t="n">
+      <c r="I71" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J71" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K71" s="8" t="s">
+      <c r="K71" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="L71" s="8" t="s">
+      <c r="L71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M71" s="9" t="n">
+      <c r="M71" s="8" t="n">
         <v>0.79</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B72" s="7" t="s">
+      <c r="A72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="8" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8" t="s">
+      <c r="E72" s="7"/>
+      <c r="F72" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8" t="s">
+      <c r="G72" s="7"/>
+      <c r="H72" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I72" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="9" t="n">
+      <c r="I72" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J72" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K72" s="8" t="s">
+      <c r="K72" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="L72" s="8" t="s">
+      <c r="L72" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M72" s="9"/>
+      <c r="M72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="7" t="s">
+      <c r="A73" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="8" t="s">
+      <c r="C73" s="6"/>
+      <c r="D73" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8" t="s">
+      <c r="E73" s="7"/>
+      <c r="F73" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8" t="s">
+      <c r="G73" s="7"/>
+      <c r="H73" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I73" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="9" t="n">
+      <c r="I73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K73" s="8" t="s">
+      <c r="K73" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="L73" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M73" s="9"/>
+      <c r="L73" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="7" t="s">
+      <c r="A74" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="8" t="s">
+      <c r="C74" s="6"/>
+      <c r="D74" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8" t="s">
+      <c r="E74" s="7"/>
+      <c r="F74" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8" t="s">
+      <c r="G74" s="7"/>
+      <c r="H74" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I74" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J74" s="9" t="n">
+      <c r="I74" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J74" s="8" t="n">
         <v>0.79</v>
       </c>
-      <c r="K74" s="8" t="s">
+      <c r="K74" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="L74" s="8" t="s">
+      <c r="L74" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M74" s="9"/>
+      <c r="M74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="8" t="s">
+      <c r="C75" s="6"/>
+      <c r="D75" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8" t="s">
+      <c r="E75" s="7"/>
+      <c r="F75" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8" t="s">
+      <c r="G75" s="7"/>
+      <c r="H75" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="I75" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J75" s="9" t="n">
+      <c r="I75" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" s="8" t="n">
         <v>2.35</v>
       </c>
-      <c r="K75" s="8" t="s">
+      <c r="K75" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="L75" s="8" t="s">
+      <c r="L75" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="M75" s="9" t="n">
+      <c r="M75" s="8" t="n">
         <v>2.35</v>
       </c>
     </row>
@@ -3655,446 +3651,446 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="14" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="14" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="14" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="14" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="14" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="14" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="14" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="14" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="60.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="14" t="s">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="14" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14" t="s">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="14" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="77.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="14" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="11"/>
+      <c r="B32" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>